<commit_message>
Restore Rentals tab to state from 3 hours ago (simple project-based filtering, original table structure)
</commit_message>
<xml_diff>
--- a/Data/Rentals/Acacia_rentals.xlsx
+++ b/Data/Rentals/Acacia_rentals.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/levan/Documents/MegaValuationer/Data/Rentals/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E26CFF60-73FC-B642-86B8-D4FCDCEF2930}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1D6AC5F-1ECC-7748-8EFA-CD9BC7287765}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="18360" xr2:uid="{F11F608D-A0BF-684C-B6F5-C2FF1ECE40B5}"/>
   </bookViews>
@@ -776,9 +776,6 @@
     <t>Community/Building</t>
   </si>
   <si>
-    <t>Sub Community / Building</t>
-  </si>
-  <si>
     <t>Beds</t>
   </si>
   <si>
@@ -810,6 +807,9 @@
   </si>
   <si>
     <t>Park Heights</t>
+  </si>
+  <si>
+    <t>Sub Community/Building</t>
   </si>
 </sst>
 </file>
@@ -1185,7 +1185,7 @@
   <dimension ref="A1:O308"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1221,37 +1221,37 @@
         <v>244</v>
       </c>
       <c r="E1" t="s">
+        <v>256</v>
+      </c>
+      <c r="F1" t="s">
         <v>245</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>246</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>247</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>248</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>249</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>250</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>251</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>252</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>253</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>254</v>
-      </c>
-      <c r="O1" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
@@ -1265,7 +1265,7 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E2" t="s">
         <v>4</v>
@@ -1312,7 +1312,7 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E3" t="s">
         <v>8</v>
@@ -1359,7 +1359,7 @@
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
@@ -1406,7 +1406,7 @@
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E5" t="s">
         <v>10</v>
@@ -1453,7 +1453,7 @@
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E6" t="s">
         <v>4</v>
@@ -1500,7 +1500,7 @@
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E7" t="s">
         <v>4</v>
@@ -1547,7 +1547,7 @@
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
@@ -1594,7 +1594,7 @@
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E9" t="s">
         <v>8</v>
@@ -1641,7 +1641,7 @@
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E10" t="s">
         <v>8</v>
@@ -1688,7 +1688,7 @@
         <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E11" t="s">
         <v>4</v>
@@ -1735,7 +1735,7 @@
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E12" t="s">
         <v>10</v>
@@ -1782,7 +1782,7 @@
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E13" t="s">
         <v>10</v>
@@ -1829,7 +1829,7 @@
         <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E14" t="s">
         <v>8</v>
@@ -1876,7 +1876,7 @@
         <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E15" t="s">
         <v>4</v>
@@ -1923,7 +1923,7 @@
         <v>2</v>
       </c>
       <c r="D16" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E16" t="s">
         <v>10</v>
@@ -1970,7 +1970,7 @@
         <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E17" t="s">
         <v>4</v>
@@ -2017,7 +2017,7 @@
         <v>2</v>
       </c>
       <c r="D18" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E18" t="s">
         <v>10</v>
@@ -2064,7 +2064,7 @@
         <v>2</v>
       </c>
       <c r="D19" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E19" t="s">
         <v>10</v>
@@ -2111,7 +2111,7 @@
         <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E20" t="s">
         <v>10</v>
@@ -2158,7 +2158,7 @@
         <v>2</v>
       </c>
       <c r="D21" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E21" t="s">
         <v>4</v>
@@ -2205,7 +2205,7 @@
         <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E22" t="s">
         <v>4</v>
@@ -2252,7 +2252,7 @@
         <v>2</v>
       </c>
       <c r="D23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E23" t="s">
         <v>8</v>
@@ -2299,7 +2299,7 @@
         <v>2</v>
       </c>
       <c r="D24" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E24" t="s">
         <v>4</v>
@@ -2346,7 +2346,7 @@
         <v>2</v>
       </c>
       <c r="D25" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E25" t="s">
         <v>8</v>
@@ -2393,7 +2393,7 @@
         <v>2</v>
       </c>
       <c r="D26" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E26" t="s">
         <v>8</v>
@@ -2440,7 +2440,7 @@
         <v>2</v>
       </c>
       <c r="D27" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E27" t="s">
         <v>10</v>
@@ -2487,7 +2487,7 @@
         <v>2</v>
       </c>
       <c r="D28" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E28" t="s">
         <v>10</v>
@@ -2534,7 +2534,7 @@
         <v>2</v>
       </c>
       <c r="D29" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E29" t="s">
         <v>8</v>
@@ -2581,7 +2581,7 @@
         <v>2</v>
       </c>
       <c r="D30" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E30" t="s">
         <v>4</v>
@@ -2628,7 +2628,7 @@
         <v>2</v>
       </c>
       <c r="D31" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E31" t="s">
         <v>4</v>
@@ -2675,7 +2675,7 @@
         <v>2</v>
       </c>
       <c r="D32" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E32" t="s">
         <v>4</v>
@@ -2722,7 +2722,7 @@
         <v>2</v>
       </c>
       <c r="D33" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E33" t="s">
         <v>4</v>
@@ -2769,7 +2769,7 @@
         <v>2</v>
       </c>
       <c r="D34" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E34" t="s">
         <v>8</v>
@@ -2816,7 +2816,7 @@
         <v>2</v>
       </c>
       <c r="D35" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E35" t="s">
         <v>8</v>
@@ -2863,7 +2863,7 @@
         <v>2</v>
       </c>
       <c r="D36" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E36" t="s">
         <v>4</v>
@@ -2910,7 +2910,7 @@
         <v>2</v>
       </c>
       <c r="D37" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E37" t="s">
         <v>4</v>
@@ -2957,7 +2957,7 @@
         <v>2</v>
       </c>
       <c r="D38" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E38" t="s">
         <v>8</v>
@@ -3004,7 +3004,7 @@
         <v>2</v>
       </c>
       <c r="D39" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E39" t="s">
         <v>4</v>
@@ -3051,7 +3051,7 @@
         <v>2</v>
       </c>
       <c r="D40" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E40" t="s">
         <v>8</v>
@@ -3098,7 +3098,7 @@
         <v>2</v>
       </c>
       <c r="D41" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E41" t="s">
         <v>8</v>
@@ -3145,7 +3145,7 @@
         <v>2</v>
       </c>
       <c r="D42" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E42" t="s">
         <v>4</v>
@@ -3192,7 +3192,7 @@
         <v>2</v>
       </c>
       <c r="D43" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E43" t="s">
         <v>10</v>
@@ -3239,7 +3239,7 @@
         <v>2</v>
       </c>
       <c r="D44" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F44" t="s">
         <v>5</v>
@@ -3283,7 +3283,7 @@
         <v>2</v>
       </c>
       <c r="D45" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E45" t="s">
         <v>8</v>
@@ -3330,7 +3330,7 @@
         <v>2</v>
       </c>
       <c r="D46" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E46" t="s">
         <v>8</v>
@@ -3377,7 +3377,7 @@
         <v>2</v>
       </c>
       <c r="D47" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E47" t="s">
         <v>4</v>
@@ -3424,7 +3424,7 @@
         <v>2</v>
       </c>
       <c r="D48" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E48" t="s">
         <v>8</v>
@@ -3471,7 +3471,7 @@
         <v>2</v>
       </c>
       <c r="D49" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E49" t="s">
         <v>10</v>
@@ -3518,7 +3518,7 @@
         <v>2</v>
       </c>
       <c r="D50" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E50" t="s">
         <v>8</v>
@@ -3565,7 +3565,7 @@
         <v>2</v>
       </c>
       <c r="D51" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E51" t="s">
         <v>10</v>
@@ -3612,7 +3612,7 @@
         <v>2</v>
       </c>
       <c r="D52" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E52" t="s">
         <v>4</v>
@@ -3659,7 +3659,7 @@
         <v>2</v>
       </c>
       <c r="D53" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E53" t="s">
         <v>10</v>
@@ -3706,7 +3706,7 @@
         <v>2</v>
       </c>
       <c r="D54" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E54" t="s">
         <v>10</v>
@@ -3753,7 +3753,7 @@
         <v>2</v>
       </c>
       <c r="D55" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F55" t="s">
         <v>5</v>
@@ -3794,7 +3794,7 @@
         <v>2</v>
       </c>
       <c r="D56" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E56" t="s">
         <v>8</v>
@@ -3841,7 +3841,7 @@
         <v>2</v>
       </c>
       <c r="D57" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E57" t="s">
         <v>4</v>
@@ -3888,7 +3888,7 @@
         <v>2</v>
       </c>
       <c r="D58" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E58" t="s">
         <v>8</v>
@@ -3935,7 +3935,7 @@
         <v>2</v>
       </c>
       <c r="D59" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E59" t="s">
         <v>10</v>
@@ -3982,7 +3982,7 @@
         <v>2</v>
       </c>
       <c r="D60" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E60" t="s">
         <v>8</v>
@@ -4029,7 +4029,7 @@
         <v>2</v>
       </c>
       <c r="D61" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E61" t="s">
         <v>8</v>
@@ -4076,7 +4076,7 @@
         <v>2</v>
       </c>
       <c r="D62" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E62" t="s">
         <v>4</v>
@@ -4123,7 +4123,7 @@
         <v>2</v>
       </c>
       <c r="D63" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E63" t="s">
         <v>8</v>
@@ -4170,7 +4170,7 @@
         <v>2</v>
       </c>
       <c r="D64" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E64" t="s">
         <v>8</v>
@@ -4217,7 +4217,7 @@
         <v>2</v>
       </c>
       <c r="D65" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E65" t="s">
         <v>4</v>
@@ -4264,7 +4264,7 @@
         <v>2</v>
       </c>
       <c r="D66" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E66" t="s">
         <v>4</v>
@@ -4311,7 +4311,7 @@
         <v>2</v>
       </c>
       <c r="D67" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E67" t="s">
         <v>10</v>
@@ -4358,7 +4358,7 @@
         <v>2</v>
       </c>
       <c r="D68" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E68" t="s">
         <v>10</v>
@@ -4405,7 +4405,7 @@
         <v>2</v>
       </c>
       <c r="D69" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E69" t="s">
         <v>4</v>
@@ -4452,7 +4452,7 @@
         <v>2</v>
       </c>
       <c r="D70" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E70" t="s">
         <v>8</v>
@@ -4499,7 +4499,7 @@
         <v>2</v>
       </c>
       <c r="D71" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E71" t="s">
         <v>8</v>
@@ -4546,7 +4546,7 @@
         <v>2</v>
       </c>
       <c r="D72" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E72" t="s">
         <v>8</v>
@@ -4593,7 +4593,7 @@
         <v>2</v>
       </c>
       <c r="D73" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E73" t="s">
         <v>8</v>
@@ -4640,7 +4640,7 @@
         <v>2</v>
       </c>
       <c r="D74" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E74" t="s">
         <v>8</v>
@@ -4687,7 +4687,7 @@
         <v>2</v>
       </c>
       <c r="D75" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E75" t="s">
         <v>4</v>
@@ -4734,7 +4734,7 @@
         <v>2</v>
       </c>
       <c r="D76" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E76" t="s">
         <v>8</v>
@@ -4781,7 +4781,7 @@
         <v>2</v>
       </c>
       <c r="D77" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E77" t="s">
         <v>8</v>
@@ -4828,7 +4828,7 @@
         <v>2</v>
       </c>
       <c r="D78" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E78" t="s">
         <v>10</v>
@@ -4875,7 +4875,7 @@
         <v>2</v>
       </c>
       <c r="D79" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E79" t="s">
         <v>10</v>
@@ -4922,7 +4922,7 @@
         <v>2</v>
       </c>
       <c r="D80" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E80" t="s">
         <v>4</v>
@@ -4969,7 +4969,7 @@
         <v>2</v>
       </c>
       <c r="D81" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E81" t="s">
         <v>4</v>
@@ -5016,7 +5016,7 @@
         <v>2</v>
       </c>
       <c r="D82" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E82" t="s">
         <v>10</v>
@@ -5063,7 +5063,7 @@
         <v>2</v>
       </c>
       <c r="D83" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E83" t="s">
         <v>4</v>
@@ -5110,7 +5110,7 @@
         <v>2</v>
       </c>
       <c r="D84" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E84" t="s">
         <v>4</v>
@@ -5157,7 +5157,7 @@
         <v>2</v>
       </c>
       <c r="D85" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E85" t="s">
         <v>10</v>
@@ -5204,7 +5204,7 @@
         <v>2</v>
       </c>
       <c r="D86" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E86" t="s">
         <v>8</v>
@@ -5251,7 +5251,7 @@
         <v>2</v>
       </c>
       <c r="D87" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E87" t="s">
         <v>8</v>
@@ -5298,7 +5298,7 @@
         <v>2</v>
       </c>
       <c r="D88" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E88" t="s">
         <v>8</v>
@@ -5345,7 +5345,7 @@
         <v>2</v>
       </c>
       <c r="D89" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E89" t="s">
         <v>8</v>
@@ -5392,7 +5392,7 @@
         <v>2</v>
       </c>
       <c r="D90" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E90" t="s">
         <v>8</v>
@@ -5439,7 +5439,7 @@
         <v>2</v>
       </c>
       <c r="D91" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E91" t="s">
         <v>8</v>
@@ -5486,7 +5486,7 @@
         <v>2</v>
       </c>
       <c r="D92" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E92" t="s">
         <v>10</v>
@@ -5533,7 +5533,7 @@
         <v>2</v>
       </c>
       <c r="D93" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E93" t="s">
         <v>4</v>
@@ -5580,7 +5580,7 @@
         <v>2</v>
       </c>
       <c r="D94" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E94" t="s">
         <v>8</v>
@@ -5627,7 +5627,7 @@
         <v>2</v>
       </c>
       <c r="D95" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E95" t="s">
         <v>8</v>
@@ -5674,7 +5674,7 @@
         <v>2</v>
       </c>
       <c r="D96" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E96" t="s">
         <v>8</v>
@@ -5721,7 +5721,7 @@
         <v>2</v>
       </c>
       <c r="D97" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E97" t="s">
         <v>4</v>
@@ -5768,7 +5768,7 @@
         <v>2</v>
       </c>
       <c r="D98" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E98" t="s">
         <v>8</v>
@@ -5815,7 +5815,7 @@
         <v>2</v>
       </c>
       <c r="D99" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E99" t="s">
         <v>4</v>
@@ -5862,7 +5862,7 @@
         <v>2</v>
       </c>
       <c r="D100" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E100" t="s">
         <v>4</v>
@@ -5909,7 +5909,7 @@
         <v>2</v>
       </c>
       <c r="D101" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E101" t="s">
         <v>4</v>
@@ -5956,7 +5956,7 @@
         <v>2</v>
       </c>
       <c r="D102" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E102" t="s">
         <v>8</v>
@@ -6003,7 +6003,7 @@
         <v>2</v>
       </c>
       <c r="D103" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E103" t="s">
         <v>10</v>
@@ -6050,7 +6050,7 @@
         <v>2</v>
       </c>
       <c r="D104" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E104" t="s">
         <v>10</v>
@@ -6097,7 +6097,7 @@
         <v>2</v>
       </c>
       <c r="D105" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E105" t="s">
         <v>10</v>
@@ -6144,7 +6144,7 @@
         <v>2</v>
       </c>
       <c r="D106" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E106" t="s">
         <v>10</v>
@@ -6191,7 +6191,7 @@
         <v>2</v>
       </c>
       <c r="D107" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E107" t="s">
         <v>8</v>
@@ -6238,7 +6238,7 @@
         <v>2</v>
       </c>
       <c r="D108" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E108" t="s">
         <v>8</v>
@@ -6285,7 +6285,7 @@
         <v>2</v>
       </c>
       <c r="D109" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E109" t="s">
         <v>10</v>
@@ -6332,7 +6332,7 @@
         <v>2</v>
       </c>
       <c r="D110" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E110" t="s">
         <v>8</v>
@@ -6379,7 +6379,7 @@
         <v>2</v>
       </c>
       <c r="D111" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E111" t="s">
         <v>4</v>
@@ -6426,7 +6426,7 @@
         <v>2</v>
       </c>
       <c r="D112" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E112" t="s">
         <v>4</v>
@@ -6473,7 +6473,7 @@
         <v>2</v>
       </c>
       <c r="D113" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E113" t="s">
         <v>8</v>
@@ -6520,7 +6520,7 @@
         <v>2</v>
       </c>
       <c r="D114" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E114" t="s">
         <v>10</v>
@@ -6567,7 +6567,7 @@
         <v>2</v>
       </c>
       <c r="D115" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E115" t="s">
         <v>10</v>
@@ -6614,7 +6614,7 @@
         <v>2</v>
       </c>
       <c r="D116" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E116" t="s">
         <v>10</v>
@@ -6661,7 +6661,7 @@
         <v>2</v>
       </c>
       <c r="D117" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E117" t="s">
         <v>8</v>
@@ -6708,7 +6708,7 @@
         <v>2</v>
       </c>
       <c r="D118" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E118" t="s">
         <v>4</v>
@@ -6755,7 +6755,7 @@
         <v>2</v>
       </c>
       <c r="D119" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E119" t="s">
         <v>4</v>
@@ -6802,7 +6802,7 @@
         <v>2</v>
       </c>
       <c r="D120" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E120" t="s">
         <v>4</v>
@@ -6849,7 +6849,7 @@
         <v>2</v>
       </c>
       <c r="D121" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E121" t="s">
         <v>8</v>
@@ -6896,7 +6896,7 @@
         <v>2</v>
       </c>
       <c r="D122" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F122" t="s">
         <v>5</v>
@@ -6937,7 +6937,7 @@
         <v>2</v>
       </c>
       <c r="D123" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E123" t="s">
         <v>10</v>
@@ -6984,7 +6984,7 @@
         <v>2</v>
       </c>
       <c r="D124" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E124" t="s">
         <v>10</v>
@@ -7031,7 +7031,7 @@
         <v>2</v>
       </c>
       <c r="D125" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E125" t="s">
         <v>4</v>
@@ -7078,7 +7078,7 @@
         <v>2</v>
       </c>
       <c r="D126" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E126" t="s">
         <v>4</v>
@@ -7125,7 +7125,7 @@
         <v>2</v>
       </c>
       <c r="D127" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E127" t="s">
         <v>8</v>
@@ -7172,7 +7172,7 @@
         <v>2</v>
       </c>
       <c r="D128" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E128" t="s">
         <v>10</v>
@@ -7219,7 +7219,7 @@
         <v>2</v>
       </c>
       <c r="D129" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E129" t="s">
         <v>10</v>
@@ -7266,7 +7266,7 @@
         <v>2</v>
       </c>
       <c r="D130" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E130" t="s">
         <v>10</v>
@@ -7313,7 +7313,7 @@
         <v>2</v>
       </c>
       <c r="D131" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E131" t="s">
         <v>4</v>
@@ -7360,7 +7360,7 @@
         <v>2</v>
       </c>
       <c r="D132" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E132" t="s">
         <v>10</v>
@@ -7407,7 +7407,7 @@
         <v>2</v>
       </c>
       <c r="D133" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E133" t="s">
         <v>10</v>
@@ -7454,7 +7454,7 @@
         <v>2</v>
       </c>
       <c r="D134" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E134" t="s">
         <v>10</v>
@@ -7501,7 +7501,7 @@
         <v>2</v>
       </c>
       <c r="D135" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E135" t="s">
         <v>8</v>
@@ -7548,7 +7548,7 @@
         <v>2</v>
       </c>
       <c r="D136" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E136" t="s">
         <v>8</v>
@@ -7595,7 +7595,7 @@
         <v>2</v>
       </c>
       <c r="D137" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E137" t="s">
         <v>10</v>
@@ -7642,7 +7642,7 @@
         <v>2</v>
       </c>
       <c r="D138" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E138" t="s">
         <v>10</v>
@@ -7689,7 +7689,7 @@
         <v>2</v>
       </c>
       <c r="D139" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E139" t="s">
         <v>8</v>
@@ -7736,7 +7736,7 @@
         <v>2</v>
       </c>
       <c r="D140" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E140" t="s">
         <v>10</v>
@@ -7783,7 +7783,7 @@
         <v>2</v>
       </c>
       <c r="D141" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E141" t="s">
         <v>8</v>
@@ -7830,7 +7830,7 @@
         <v>2</v>
       </c>
       <c r="D142" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E142" t="s">
         <v>8</v>
@@ -7877,7 +7877,7 @@
         <v>2</v>
       </c>
       <c r="D143" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E143" t="s">
         <v>4</v>
@@ -7924,7 +7924,7 @@
         <v>2</v>
       </c>
       <c r="D144" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E144" t="s">
         <v>10</v>
@@ -7971,7 +7971,7 @@
         <v>2</v>
       </c>
       <c r="D145" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E145" t="s">
         <v>8</v>
@@ -8018,7 +8018,7 @@
         <v>2</v>
       </c>
       <c r="D146" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E146" t="s">
         <v>8</v>
@@ -8065,7 +8065,7 @@
         <v>2</v>
       </c>
       <c r="D147" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E147" t="s">
         <v>4</v>
@@ -8112,7 +8112,7 @@
         <v>2</v>
       </c>
       <c r="D148" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E148" t="s">
         <v>4</v>
@@ -8159,7 +8159,7 @@
         <v>2</v>
       </c>
       <c r="D149" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E149" t="s">
         <v>4</v>
@@ -8206,7 +8206,7 @@
         <v>2</v>
       </c>
       <c r="D150" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E150" t="s">
         <v>8</v>
@@ -8253,7 +8253,7 @@
         <v>2</v>
       </c>
       <c r="D151" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E151" t="s">
         <v>8</v>
@@ -8300,7 +8300,7 @@
         <v>2</v>
       </c>
       <c r="D152" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E152" t="s">
         <v>8</v>
@@ -8347,7 +8347,7 @@
         <v>2</v>
       </c>
       <c r="D153" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E153" t="s">
         <v>8</v>
@@ -8394,7 +8394,7 @@
         <v>2</v>
       </c>
       <c r="D154" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E154" t="s">
         <v>8</v>
@@ -8441,7 +8441,7 @@
         <v>2</v>
       </c>
       <c r="D155" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E155" t="s">
         <v>8</v>
@@ -8488,7 +8488,7 @@
         <v>2</v>
       </c>
       <c r="D156" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E156" t="s">
         <v>10</v>
@@ -8535,7 +8535,7 @@
         <v>2</v>
       </c>
       <c r="D157" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E157" t="s">
         <v>4</v>
@@ -8582,7 +8582,7 @@
         <v>2</v>
       </c>
       <c r="D158" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E158" t="s">
         <v>8</v>
@@ -8629,7 +8629,7 @@
         <v>2</v>
       </c>
       <c r="D159" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E159" t="s">
         <v>4</v>
@@ -8676,7 +8676,7 @@
         <v>2</v>
       </c>
       <c r="D160" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E160" t="s">
         <v>10</v>
@@ -8723,7 +8723,7 @@
         <v>2</v>
       </c>
       <c r="D161" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E161" t="s">
         <v>4</v>
@@ -8770,7 +8770,7 @@
         <v>2</v>
       </c>
       <c r="D162" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E162" t="s">
         <v>8</v>
@@ -8817,7 +8817,7 @@
         <v>2</v>
       </c>
       <c r="D163" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E163" t="s">
         <v>4</v>
@@ -8864,7 +8864,7 @@
         <v>2</v>
       </c>
       <c r="D164" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E164" t="s">
         <v>8</v>
@@ -8911,7 +8911,7 @@
         <v>2</v>
       </c>
       <c r="D165" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E165" t="s">
         <v>8</v>
@@ -8958,7 +8958,7 @@
         <v>2</v>
       </c>
       <c r="D166" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E166" t="s">
         <v>4</v>
@@ -9005,7 +9005,7 @@
         <v>2</v>
       </c>
       <c r="D167" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E167" t="s">
         <v>10</v>
@@ -9052,7 +9052,7 @@
         <v>2</v>
       </c>
       <c r="D168" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E168" t="s">
         <v>8</v>
@@ -9099,7 +9099,7 @@
         <v>2</v>
       </c>
       <c r="D169" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E169" t="s">
         <v>8</v>
@@ -9146,7 +9146,7 @@
         <v>2</v>
       </c>
       <c r="D170" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E170" t="s">
         <v>8</v>
@@ -9193,7 +9193,7 @@
         <v>2</v>
       </c>
       <c r="D171" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E171" t="s">
         <v>10</v>
@@ -9240,7 +9240,7 @@
         <v>2</v>
       </c>
       <c r="D172" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E172" t="s">
         <v>8</v>
@@ -9287,7 +9287,7 @@
         <v>2</v>
       </c>
       <c r="D173" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E173" t="s">
         <v>8</v>
@@ -9334,7 +9334,7 @@
         <v>2</v>
       </c>
       <c r="D174" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E174" t="s">
         <v>10</v>
@@ -9381,7 +9381,7 @@
         <v>2</v>
       </c>
       <c r="D175" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E175" t="s">
         <v>8</v>
@@ -9428,7 +9428,7 @@
         <v>2</v>
       </c>
       <c r="D176" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E176" t="s">
         <v>8</v>
@@ -9475,7 +9475,7 @@
         <v>2</v>
       </c>
       <c r="D177" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E177" t="s">
         <v>4</v>
@@ -9522,7 +9522,7 @@
         <v>2</v>
       </c>
       <c r="D178" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E178" t="s">
         <v>10</v>
@@ -9569,7 +9569,7 @@
         <v>2</v>
       </c>
       <c r="D179" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E179" t="s">
         <v>4</v>
@@ -9616,7 +9616,7 @@
         <v>2</v>
       </c>
       <c r="D180" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E180" t="s">
         <v>10</v>
@@ -9663,7 +9663,7 @@
         <v>2</v>
       </c>
       <c r="D181" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E181" t="s">
         <v>4</v>
@@ -9710,7 +9710,7 @@
         <v>2</v>
       </c>
       <c r="D182" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E182" t="s">
         <v>8</v>
@@ -9757,7 +9757,7 @@
         <v>2</v>
       </c>
       <c r="D183" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E183" t="s">
         <v>8</v>
@@ -9804,7 +9804,7 @@
         <v>2</v>
       </c>
       <c r="D184" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E184" t="s">
         <v>8</v>
@@ -9851,7 +9851,7 @@
         <v>2</v>
       </c>
       <c r="D185" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E185" t="s">
         <v>10</v>
@@ -9898,7 +9898,7 @@
         <v>2</v>
       </c>
       <c r="D186" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E186" t="s">
         <v>4</v>
@@ -9945,7 +9945,7 @@
         <v>2</v>
       </c>
       <c r="D187" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E187" t="s">
         <v>4</v>
@@ -9992,7 +9992,7 @@
         <v>2</v>
       </c>
       <c r="D188" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E188" t="s">
         <v>10</v>
@@ -10039,7 +10039,7 @@
         <v>2</v>
       </c>
       <c r="D189" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F189" t="s">
         <v>5</v>
@@ -10083,7 +10083,7 @@
         <v>2</v>
       </c>
       <c r="D190" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E190" t="s">
         <v>4</v>
@@ -10130,7 +10130,7 @@
         <v>2</v>
       </c>
       <c r="D191" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E191" t="s">
         <v>4</v>
@@ -10177,7 +10177,7 @@
         <v>2</v>
       </c>
       <c r="D192" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E192" t="s">
         <v>4</v>
@@ -10224,7 +10224,7 @@
         <v>2</v>
       </c>
       <c r="D193" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E193" t="s">
         <v>10</v>
@@ -10271,7 +10271,7 @@
         <v>2</v>
       </c>
       <c r="D194" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E194" t="s">
         <v>4</v>
@@ -10318,7 +10318,7 @@
         <v>2</v>
       </c>
       <c r="D195" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E195" t="s">
         <v>8</v>
@@ -10365,7 +10365,7 @@
         <v>2</v>
       </c>
       <c r="D196" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E196" t="s">
         <v>4</v>
@@ -10412,7 +10412,7 @@
         <v>2</v>
       </c>
       <c r="D197" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F197" t="s">
         <v>5</v>
@@ -10456,7 +10456,7 @@
         <v>2</v>
       </c>
       <c r="D198" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E198" t="s">
         <v>10</v>
@@ -10503,7 +10503,7 @@
         <v>2</v>
       </c>
       <c r="D199" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E199" t="s">
         <v>4</v>
@@ -10550,7 +10550,7 @@
         <v>2</v>
       </c>
       <c r="D200" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E200" t="s">
         <v>8</v>
@@ -10597,7 +10597,7 @@
         <v>2</v>
       </c>
       <c r="D201" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E201" t="s">
         <v>10</v>
@@ -10644,7 +10644,7 @@
         <v>2</v>
       </c>
       <c r="D202" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E202" t="s">
         <v>4</v>
@@ -10691,7 +10691,7 @@
         <v>2</v>
       </c>
       <c r="D203" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E203" t="s">
         <v>4</v>
@@ -10738,7 +10738,7 @@
         <v>2</v>
       </c>
       <c r="D204" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E204" t="s">
         <v>10</v>
@@ -10785,7 +10785,7 @@
         <v>2</v>
       </c>
       <c r="D205" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E205" t="s">
         <v>4</v>
@@ -10832,7 +10832,7 @@
         <v>2</v>
       </c>
       <c r="D206" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E206" t="s">
         <v>8</v>
@@ -10879,7 +10879,7 @@
         <v>2</v>
       </c>
       <c r="D207" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E207" t="s">
         <v>4</v>
@@ -10926,7 +10926,7 @@
         <v>2</v>
       </c>
       <c r="D208" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E208" t="s">
         <v>4</v>
@@ -10973,7 +10973,7 @@
         <v>2</v>
       </c>
       <c r="D209" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E209" t="s">
         <v>10</v>
@@ -11020,7 +11020,7 @@
         <v>2</v>
       </c>
       <c r="D210" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E210" t="s">
         <v>8</v>
@@ -11067,7 +11067,7 @@
         <v>2</v>
       </c>
       <c r="D211" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E211" t="s">
         <v>4</v>
@@ -11114,7 +11114,7 @@
         <v>2</v>
       </c>
       <c r="D212" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E212" t="s">
         <v>4</v>
@@ -11161,7 +11161,7 @@
         <v>2</v>
       </c>
       <c r="D213" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E213" t="s">
         <v>4</v>
@@ -11208,7 +11208,7 @@
         <v>2</v>
       </c>
       <c r="D214" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E214" t="s">
         <v>10</v>
@@ -11255,7 +11255,7 @@
         <v>2</v>
       </c>
       <c r="D215" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E215" t="s">
         <v>8</v>
@@ -11302,7 +11302,7 @@
         <v>2</v>
       </c>
       <c r="D216" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E216" t="s">
         <v>10</v>
@@ -11349,7 +11349,7 @@
         <v>2</v>
       </c>
       <c r="D217" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E217" t="s">
         <v>4</v>
@@ -11396,7 +11396,7 @@
         <v>2</v>
       </c>
       <c r="D218" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E218" t="s">
         <v>4</v>
@@ -11443,7 +11443,7 @@
         <v>2</v>
       </c>
       <c r="D219" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E219" t="s">
         <v>10</v>
@@ -11490,7 +11490,7 @@
         <v>2</v>
       </c>
       <c r="D220" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E220" t="s">
         <v>8</v>
@@ -11537,7 +11537,7 @@
         <v>2</v>
       </c>
       <c r="D221" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E221" t="s">
         <v>4</v>
@@ -11584,7 +11584,7 @@
         <v>2</v>
       </c>
       <c r="D222" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E222" t="s">
         <v>4</v>
@@ -11631,7 +11631,7 @@
         <v>2</v>
       </c>
       <c r="D223" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E223" t="s">
         <v>8</v>
@@ -11678,7 +11678,7 @@
         <v>2</v>
       </c>
       <c r="D224" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E224" t="s">
         <v>8</v>
@@ -11725,7 +11725,7 @@
         <v>2</v>
       </c>
       <c r="D225" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E225" t="s">
         <v>10</v>
@@ -11772,7 +11772,7 @@
         <v>2</v>
       </c>
       <c r="D226" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E226" t="s">
         <v>10</v>
@@ -11819,7 +11819,7 @@
         <v>2</v>
       </c>
       <c r="D227" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E227" t="s">
         <v>10</v>
@@ -11866,7 +11866,7 @@
         <v>2</v>
       </c>
       <c r="D228" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E228" t="s">
         <v>4</v>
@@ -11913,7 +11913,7 @@
         <v>2</v>
       </c>
       <c r="D229" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E229" t="s">
         <v>4</v>
@@ -11960,7 +11960,7 @@
         <v>2</v>
       </c>
       <c r="D230" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E230" t="s">
         <v>4</v>
@@ -12007,7 +12007,7 @@
         <v>2</v>
       </c>
       <c r="D231" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E231" t="s">
         <v>4</v>
@@ -12054,7 +12054,7 @@
         <v>2</v>
       </c>
       <c r="D232" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E232" t="s">
         <v>4</v>
@@ -12101,7 +12101,7 @@
         <v>2</v>
       </c>
       <c r="D233" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E233" t="s">
         <v>8</v>
@@ -12148,7 +12148,7 @@
         <v>2</v>
       </c>
       <c r="D234" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E234" t="s">
         <v>4</v>
@@ -12195,7 +12195,7 @@
         <v>2</v>
       </c>
       <c r="D235" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E235" t="s">
         <v>4</v>
@@ -12242,7 +12242,7 @@
         <v>2</v>
       </c>
       <c r="D236" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E236" t="s">
         <v>4</v>
@@ -12289,7 +12289,7 @@
         <v>2</v>
       </c>
       <c r="D237" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E237" t="s">
         <v>8</v>
@@ -12336,7 +12336,7 @@
         <v>2</v>
       </c>
       <c r="D238" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E238" t="s">
         <v>8</v>
@@ -12383,7 +12383,7 @@
         <v>2</v>
       </c>
       <c r="D239" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E239" t="s">
         <v>10</v>
@@ -12430,7 +12430,7 @@
         <v>2</v>
       </c>
       <c r="D240" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E240" t="s">
         <v>8</v>
@@ -12477,7 +12477,7 @@
         <v>2</v>
       </c>
       <c r="D241" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E241" t="s">
         <v>10</v>
@@ -12524,7 +12524,7 @@
         <v>2</v>
       </c>
       <c r="D242" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E242" t="s">
         <v>8</v>
@@ -12571,7 +12571,7 @@
         <v>2</v>
       </c>
       <c r="D243" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E243" t="s">
         <v>8</v>
@@ -12618,7 +12618,7 @@
         <v>2</v>
       </c>
       <c r="D244" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E244" t="s">
         <v>8</v>
@@ -12665,7 +12665,7 @@
         <v>2</v>
       </c>
       <c r="D245" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E245" t="s">
         <v>4</v>
@@ -12712,7 +12712,7 @@
         <v>2</v>
       </c>
       <c r="D246" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E246" t="s">
         <v>4</v>
@@ -12759,7 +12759,7 @@
         <v>2</v>
       </c>
       <c r="D247" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E247" t="s">
         <v>10</v>
@@ -12806,7 +12806,7 @@
         <v>2</v>
       </c>
       <c r="D248" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E248" t="s">
         <v>8</v>
@@ -12853,7 +12853,7 @@
         <v>2</v>
       </c>
       <c r="D249" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E249" t="s">
         <v>8</v>
@@ -12900,7 +12900,7 @@
         <v>2</v>
       </c>
       <c r="D250" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E250" t="s">
         <v>4</v>
@@ -12947,7 +12947,7 @@
         <v>2</v>
       </c>
       <c r="D251" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E251" t="s">
         <v>10</v>
@@ -12994,7 +12994,7 @@
         <v>2</v>
       </c>
       <c r="D252" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E252" t="s">
         <v>8</v>
@@ -13041,7 +13041,7 @@
         <v>2</v>
       </c>
       <c r="D253" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E253" t="s">
         <v>8</v>
@@ -13088,7 +13088,7 @@
         <v>2</v>
       </c>
       <c r="D254" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E254" t="s">
         <v>10</v>
@@ -13135,7 +13135,7 @@
         <v>2</v>
       </c>
       <c r="D255" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E255" t="s">
         <v>4</v>
@@ -13182,7 +13182,7 @@
         <v>2</v>
       </c>
       <c r="D256" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E256" t="s">
         <v>8</v>
@@ -13229,7 +13229,7 @@
         <v>2</v>
       </c>
       <c r="D257" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E257" t="s">
         <v>4</v>
@@ -13276,7 +13276,7 @@
         <v>2</v>
       </c>
       <c r="D258" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E258" t="s">
         <v>10</v>
@@ -13323,7 +13323,7 @@
         <v>2</v>
       </c>
       <c r="D259" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E259" t="s">
         <v>8</v>
@@ -13370,7 +13370,7 @@
         <v>2</v>
       </c>
       <c r="D260" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E260" t="s">
         <v>4</v>
@@ -13417,7 +13417,7 @@
         <v>2</v>
       </c>
       <c r="D261" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E261" t="s">
         <v>10</v>
@@ -13464,7 +13464,7 @@
         <v>2</v>
       </c>
       <c r="D262" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E262" t="s">
         <v>4</v>
@@ -13511,7 +13511,7 @@
         <v>2</v>
       </c>
       <c r="D263" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E263" t="s">
         <v>8</v>
@@ -13558,7 +13558,7 @@
         <v>2</v>
       </c>
       <c r="D264" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E264" t="s">
         <v>4</v>
@@ -13605,7 +13605,7 @@
         <v>2</v>
       </c>
       <c r="D265" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E265" t="s">
         <v>8</v>
@@ -13652,7 +13652,7 @@
         <v>2</v>
       </c>
       <c r="D266" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E266" t="s">
         <v>4</v>
@@ -13699,7 +13699,7 @@
         <v>2</v>
       </c>
       <c r="D267" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E267" t="s">
         <v>8</v>
@@ -13746,7 +13746,7 @@
         <v>2</v>
       </c>
       <c r="D268" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E268" t="s">
         <v>10</v>
@@ -13793,7 +13793,7 @@
         <v>2</v>
       </c>
       <c r="D269" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E269" t="s">
         <v>8</v>
@@ -13840,7 +13840,7 @@
         <v>2</v>
       </c>
       <c r="D270" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E270" t="s">
         <v>4</v>
@@ -13887,7 +13887,7 @@
         <v>2</v>
       </c>
       <c r="D271" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E271" t="s">
         <v>8</v>
@@ -13934,7 +13934,7 @@
         <v>2</v>
       </c>
       <c r="D272" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E272" t="s">
         <v>4</v>
@@ -13981,7 +13981,7 @@
         <v>2</v>
       </c>
       <c r="D273" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E273" t="s">
         <v>4</v>
@@ -14028,7 +14028,7 @@
         <v>2</v>
       </c>
       <c r="D274" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E274" t="s">
         <v>4</v>
@@ -14075,7 +14075,7 @@
         <v>2</v>
       </c>
       <c r="D275" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E275" t="s">
         <v>8</v>
@@ -14122,7 +14122,7 @@
         <v>2</v>
       </c>
       <c r="D276" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E276" t="s">
         <v>8</v>
@@ -14169,7 +14169,7 @@
         <v>2</v>
       </c>
       <c r="D277" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E277" t="s">
         <v>8</v>
@@ -14216,7 +14216,7 @@
         <v>2</v>
       </c>
       <c r="D278" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E278" t="s">
         <v>4</v>
@@ -14263,7 +14263,7 @@
         <v>2</v>
       </c>
       <c r="D279" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E279" t="s">
         <v>4</v>
@@ -14310,7 +14310,7 @@
         <v>2</v>
       </c>
       <c r="D280" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E280" t="s">
         <v>8</v>
@@ -14357,7 +14357,7 @@
         <v>2</v>
       </c>
       <c r="D281" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E281" t="s">
         <v>8</v>
@@ -14404,7 +14404,7 @@
         <v>2</v>
       </c>
       <c r="D282" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E282" t="s">
         <v>8</v>
@@ -14451,7 +14451,7 @@
         <v>2</v>
       </c>
       <c r="D283" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E283" t="s">
         <v>8</v>
@@ -14498,7 +14498,7 @@
         <v>2</v>
       </c>
       <c r="D284" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E284" t="s">
         <v>8</v>
@@ -14545,7 +14545,7 @@
         <v>2</v>
       </c>
       <c r="D285" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E285" t="s">
         <v>8</v>
@@ -14592,7 +14592,7 @@
         <v>2</v>
       </c>
       <c r="D286" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E286" t="s">
         <v>4</v>
@@ -14639,7 +14639,7 @@
         <v>2</v>
       </c>
       <c r="D287" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E287" t="s">
         <v>8</v>
@@ -14686,7 +14686,7 @@
         <v>2</v>
       </c>
       <c r="D288" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E288" t="s">
         <v>10</v>
@@ -14733,7 +14733,7 @@
         <v>2</v>
       </c>
       <c r="D289" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E289" t="s">
         <v>8</v>
@@ -14780,7 +14780,7 @@
         <v>2</v>
       </c>
       <c r="D290" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E290" t="s">
         <v>8</v>
@@ -14827,7 +14827,7 @@
         <v>2</v>
       </c>
       <c r="D291" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E291" t="s">
         <v>8</v>
@@ -14874,7 +14874,7 @@
         <v>2</v>
       </c>
       <c r="D292" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E292" t="s">
         <v>8</v>
@@ -14921,7 +14921,7 @@
         <v>2</v>
       </c>
       <c r="D293" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E293" t="s">
         <v>8</v>
@@ -14968,7 +14968,7 @@
         <v>2</v>
       </c>
       <c r="D294" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E294" t="s">
         <v>8</v>
@@ -15015,7 +15015,7 @@
         <v>2</v>
       </c>
       <c r="D295" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E295" t="s">
         <v>4</v>
@@ -15062,7 +15062,7 @@
         <v>2</v>
       </c>
       <c r="D296" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E296" t="s">
         <v>8</v>
@@ -15109,7 +15109,7 @@
         <v>2</v>
       </c>
       <c r="D297" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E297" t="s">
         <v>8</v>
@@ -15156,7 +15156,7 @@
         <v>2</v>
       </c>
       <c r="D298" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E298" t="s">
         <v>10</v>
@@ -15203,7 +15203,7 @@
         <v>2</v>
       </c>
       <c r="D299" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E299" t="s">
         <v>4</v>
@@ -15250,7 +15250,7 @@
         <v>2</v>
       </c>
       <c r="D300" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E300" t="s">
         <v>4</v>
@@ -15297,7 +15297,7 @@
         <v>2</v>
       </c>
       <c r="D301" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E301" t="s">
         <v>8</v>
@@ -15344,7 +15344,7 @@
         <v>2</v>
       </c>
       <c r="D302" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E302" t="s">
         <v>8</v>
@@ -15391,7 +15391,7 @@
         <v>2</v>
       </c>
       <c r="D303" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E303" t="s">
         <v>10</v>
@@ -15438,7 +15438,7 @@
         <v>2</v>
       </c>
       <c r="D304" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E304" t="s">
         <v>4</v>
@@ -15485,7 +15485,7 @@
         <v>2</v>
       </c>
       <c r="D305" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E305" t="s">
         <v>8</v>
@@ -15532,7 +15532,7 @@
         <v>2</v>
       </c>
       <c r="D306" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E306" t="s">
         <v>4</v>
@@ -15579,7 +15579,7 @@
         <v>2</v>
       </c>
       <c r="D307" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E307" t="s">
         <v>8</v>
@@ -15626,7 +15626,7 @@
         <v>2</v>
       </c>
       <c r="D308" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E308" t="s">
         <v>10</v>

</xml_diff>